<commit_message>
New fields in excel with updates to python
</commit_message>
<xml_diff>
--- a/esxi-hosts.xlsx
+++ b/esxi-hosts.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tietocorporation-my.sharepoint.com/personal/onni_rautanen_tieto_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautaonn/GIT/esxipxe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{0D8874B6-26D9-4A8D-9F19-5BB55DF0E5EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D33B19A5-6946-4643-BA81-12C603356457}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AFE43B-3939-874D-8222-6382AC7FD6C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{FD2C5535-F74D-41F4-BDAC-39876CDCBDB5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{FD2C5535-F74D-41F4-BDAC-39876CDCBDB5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Hosts" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$2:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hosts!$A$2:$K$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,9 +36,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
-  <si>
-    <t>box1.oizone.net</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+  <si>
+    <t>fqdn</t>
+  </si>
+  <si>
+    <t>nic</t>
+  </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>netmask</t>
+  </si>
+  <si>
+    <t>gateway</t>
+  </si>
+  <si>
+    <t>dns</t>
+  </si>
+  <si>
+    <t>vlan</t>
+  </si>
+  <si>
+    <t>GUID</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>vmnic0</t>
+  </si>
+  <si>
+    <t>ntp(s)</t>
+  </si>
+  <si>
+    <t>HTTP Share:</t>
+  </si>
+  <si>
+    <t>Disk selection</t>
+  </si>
+  <si>
+    <t>Transparent page sharing</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>CEIP participation (0=ask, 1=yes, 2=no)</t>
+  </si>
+  <si>
+    <t>create vSAN</t>
+  </si>
+  <si>
+    <t>vSAN capacitydisk(s)</t>
   </si>
   <si>
     <t>10.0.1.21</t>
@@ -50,112 +107,70 @@
     <t>10.0.1.1</t>
   </si>
   <si>
+    <t>44454c4c-4400-1038-8043-b8c04f325232</t>
+  </si>
+  <si>
+    <t>Apacer_SM230</t>
+  </si>
+  <si>
+    <t>vcf.oizone.net</t>
+  </si>
+  <si>
+    <t>10.0.1.22</t>
+  </si>
+  <si>
+    <t>44454c4c-3700-1039-8043-b1c04f325232</t>
+  </si>
+  <si>
+    <t>10.0.1.23</t>
+  </si>
+  <si>
+    <t>44454c4c-3800-1039-8043-b4c04f325232</t>
+  </si>
+  <si>
+    <t>10.0.1.24</t>
+  </si>
+  <si>
+    <t>44454c4c-4200-1039-8043-b3c04f325232</t>
+  </si>
+  <si>
+    <t>10.0.1.7</t>
+  </si>
+  <si>
     <t>00b259ed-7772-e311-a72c-b8aeed720482</t>
   </si>
   <si>
     <t>Samsung_SSD_850_EVO_250GB</t>
   </si>
   <si>
-    <t>vmnic0</t>
-  </si>
-  <si>
-    <t>10.0.2.2,10.0.2.3</t>
-  </si>
-  <si>
-    <t>fqdn</t>
-  </si>
-  <si>
-    <t>nic</t>
-  </si>
-  <si>
-    <t>ip</t>
-  </si>
-  <si>
-    <t>netmask</t>
-  </si>
-  <si>
-    <t>gateway</t>
-  </si>
-  <si>
-    <t>dns</t>
-  </si>
-  <si>
-    <t>vlan</t>
-  </si>
-  <si>
-    <t>capacitydisk</t>
-  </si>
-  <si>
-    <t>0.fi.pool.ntp.org</t>
-  </si>
-  <si>
-    <t>1.fi.pool.ntp.org</t>
-  </si>
-  <si>
-    <t>ntp1</t>
-  </si>
-  <si>
-    <t>ntp2</t>
-  </si>
-  <si>
-    <t>GUID</t>
-  </si>
-  <si>
-    <t>44454c4c-3700-1039-8043-b1c04f325232</t>
-  </si>
-  <si>
-    <t>44454c4c-3800-1039-8043-b4c04f325232</t>
-  </si>
-  <si>
-    <t>44454c4c-4200-1039-8043-b3c04f325232</t>
-  </si>
-  <si>
-    <t>44454c4c-4400-1038-8043-b8c04f325232</t>
-  </si>
-  <si>
-    <t>nuke.oizone.net</t>
-  </si>
-  <si>
-    <t>10.0.1.7</t>
-  </si>
-  <si>
-    <t>10.0.1.22</t>
-  </si>
-  <si>
-    <t>10.0.1.23</t>
-  </si>
-  <si>
-    <t>10.0.1.24</t>
-  </si>
-  <si>
-    <t>Apacer_SM230</t>
-  </si>
-  <si>
-    <t>box2.oizone.net</t>
-  </si>
-  <si>
-    <t>box3.oizone.net</t>
-  </si>
-  <si>
-    <t>box4.oizone.net</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>vcf.oizone.net</t>
-  </si>
-  <si>
-    <t>--iscrypted $6$0lIy5uWJlPsz5SCc$vM9J7t6yuvrOSJjtiJM73kcN9uO8qahm3QJE0SVK7Xrwz0tlag9lIC/4sQw3mG.x3g5HFYmaYCSxrP4ax5i670</t>
-  </si>
-  <si>
-    <t>NFS Share:</t>
-  </si>
-  <si>
-    <t>nassikka.oizone.net/export/pxeboot</t>
+    <t>0.fi.pool.ntp.org,1.fi.pool.ntp.org</t>
+  </si>
+  <si>
+    <t>--firstdisk=usb</t>
+  </si>
+  <si>
+    <t>box1.vcf.oizone.net</t>
+  </si>
+  <si>
+    <t>box2.vcf.oizone.net</t>
+  </si>
+  <si>
+    <t>box3.vcf.oizone.net</t>
+  </si>
+  <si>
+    <t>box4.vcf.oizone.net</t>
+  </si>
+  <si>
+    <t>nuke.vcf.oizone.net</t>
+  </si>
+  <si>
+    <t>http-repo.vcf.oizone.net</t>
+  </si>
+  <si>
+    <t>62.241.198.245,62.241.198.246</t>
+  </si>
+  <si>
+    <t>P4ssw0rd</t>
   </si>
 </sst>
 </file>
@@ -523,278 +538,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498C0852-A23D-4AC6-A0A2-2AEDE18809CF}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="120.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="15" max="15" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G3">
         <v>1110</v>
       </c>
       <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>37</v>
+      <c r="P3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G4">
         <v>1110</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
         <v>16</v>
       </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>37</v>
+      <c r="P4" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G5">
         <v>1110</v>
       </c>
       <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G6">
         <v>1110</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
         <v>16</v>
       </c>
-      <c r="K6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>37</v>
+      <c r="P6" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>1110</v>
       </c>
       <c r="H7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" t="s">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
         <v>16</v>
       </c>
-      <c r="K7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>37</v>
+      <c r="P7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -805,18 +879,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1029,26 +1103,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47AAB25B-241E-441A-B096-A4CB95D95135}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D24959D-2EAF-4BA9-B124-B146F8BCEB26}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="420b1caf-0da6-4c93-b8f0-e54cf6b84b95"/>
+    <ds:schemaRef ds:uri="06fc048b-0742-4b12-8c99-f64ada4dab12"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D24959D-2EAF-4BA9-B124-B146F8BCEB26}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47AAB25B-241E-441A-B096-A4CB95D95135}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="420b1caf-0da6-4c93-b8f0-e54cf6b84b95"/>
-    <ds:schemaRef ds:uri="06fc048b-0742-4b12-8c99-f64ada4dab12"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>